<commit_message>
Updated the template according the to note tracking update. Notes are tracked for Klas2.
</commit_message>
<xml_diff>
--- a/Materiaalcontrole.xlsx
+++ b/Materiaalcontrole.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merijn\GIT\Materiaalcontrole\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626F12AD-F32E-46CA-BEA9-0ED8A4D6107C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4337F88-1102-4EF9-9157-73915F97E61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Klas1" sheetId="1" r:id="rId1"/>
-    <sheet name="Klas3" sheetId="2" r:id="rId2"/>
+    <sheet name="Klas2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Voornaam</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Voornaam20</t>
+  </si>
+  <si>
+    <t>Nota</t>
   </si>
   <si>
     <t>Name1</t>
@@ -520,9 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -701,201 +702,275 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Renamed column 'Middagstudies' to more generic 'Sancties'
</commit_message>
<xml_diff>
--- a/Materiaalcontrole.xlsx
+++ b/Materiaalcontrole.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merijn\GIT\Materiaalcontrole\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4337F88-1102-4EF9-9157-73915F97E61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94624672-8F44-4E87-B0B2-1013ABC69BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Klas1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
     <t>Voornaam</t>
   </si>
   <si>
-    <t>Middagstudies</t>
-  </si>
-  <si>
     <t>Voornaam1</t>
   </si>
   <si>
@@ -159,19 +156,27 @@
   </si>
   <si>
     <t>Name23</t>
+  </si>
+  <si>
+    <t>Sancties</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -214,8 +219,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -523,7 +531,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -531,13 +541,13 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -545,7 +555,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -553,7 +563,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -561,7 +571,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -569,7 +579,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -577,7 +587,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -585,7 +595,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -593,7 +603,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -601,7 +611,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -609,7 +619,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -617,7 +627,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -625,7 +635,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -633,7 +643,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -641,7 +651,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -649,7 +659,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -657,7 +667,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -665,7 +675,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -673,7 +683,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -681,7 +691,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -689,7 +699,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -705,7 +715,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,16 +724,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -734,7 +744,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -745,7 +755,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -756,7 +766,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -767,7 +777,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -778,7 +788,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -789,7 +799,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -800,7 +810,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -811,7 +821,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -822,7 +832,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -833,7 +843,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -844,7 +854,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -855,7 +865,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -866,7 +876,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -877,7 +887,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -888,7 +898,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -899,7 +909,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -910,7 +920,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -921,7 +931,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -932,7 +942,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -943,7 +953,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -954,7 +964,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -965,7 +975,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24">
         <v>0</v>

</xml_diff>